<commit_message>
enabled the DACOUT Plexim RT-BOX simulation works typically
</commit_message>
<xml_diff>
--- a/documentation/pin define.xlsx
+++ b/documentation/pin define.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A50807\Downloads\20250827\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\QQE_990W_Opp_3416483\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159122E6-927C-475A-A428-9E3F6BF005A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD257B30-7FE1-4BBF-966B-D59183E3C364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{CA86AAE4-556E-4F25-984B-50D9820D761B}"/>
+    <workbookView xWindow="-28920" yWindow="-2955" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CA86AAE4-556E-4F25-984B-50D9820D761B}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary" sheetId="1" r:id="rId1"/>
@@ -2374,7 +2374,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3070,8 +3070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59C81CE-0568-48AC-A368-7383C5FEE29C}">
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3254,8 +3254,12 @@
       <c r="C16" s="14" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" s="7">
+        <f>B12/B8</f>
+        <v>0.16500000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>211</v>
       </c>
@@ -3265,7 +3269,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>219</v>
       </c>
@@ -3279,7 +3283,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>220</v>
       </c>
@@ -3293,7 +3297,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>221</v>
       </c>
@@ -3307,7 +3311,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>222</v>
       </c>
@@ -3321,7 +3325,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>223</v>
       </c>
@@ -3335,7 +3339,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10"/>
       <c r="B27" s="11">
         <f>(B25*B26)/(B25+B26)</f>
@@ -3346,7 +3350,7 @@
       </c>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>213</v>
       </c>
@@ -3359,7 +3363,7 @@
       </c>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>208</v>
       </c>
@@ -3369,7 +3373,7 @@
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>209</v>
       </c>
@@ -3379,7 +3383,7 @@
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>214</v>
       </c>
@@ -3389,6 +3393,10 @@
       </c>
       <c r="C31" s="14"/>
       <c r="D31" s="10"/>
+      <c r="E31" s="7">
+        <f>B28/B5</f>
+        <v>3.5335689045936395E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>